<commit_message>
Stored functions, triggers, and data integrity testing
</commit_message>
<xml_diff>
--- a/Testing DB.xlsx
+++ b/Testing DB.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Database_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC2AE5C-8D3C-47A5-AD17-D8F1A8E373AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A544EF0-C5BE-4234-BA3E-146F94596576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E70D3E94-7E3F-464A-B5D4-DDA269FF24CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="4" xr2:uid="{E70D3E94-7E3F-464A-B5D4-DDA269FF24CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheme Testing - Tables &amp; Field" sheetId="1" r:id="rId1"/>
-    <sheet name="Stored Procedures Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="Stored Procedures ManualTesting" sheetId="2" r:id="rId2"/>
+    <sheet name="Stored Functions - TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="Triggers Testing" sheetId="4" r:id="rId4"/>
+    <sheet name="Database Integrity Testcases" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="140">
   <si>
     <t>TC ID</t>
   </si>
@@ -207,13 +210,375 @@
     <t>SELECT column_name, is_nullable
 FROM Information_scheme.columns 
 WHERE table_name = 'products';</t>
+  </si>
+  <si>
+    <t>Check stored procedures are exists in the database</t>
+  </si>
+  <si>
+    <t>Check stored procedure
+"SelectAllCustomers" display all records from the customer table</t>
+  </si>
+  <si>
+    <t>Check stored procedure
+"SelectAllCustomersByCityAndPin" by passing 'cityname' and 'pincode' as input parameters</t>
+  </si>
+  <si>
+    <t>Check stored procedure
+"get_order_by_cust" by passing 'custId' as input parameter</t>
+  </si>
+  <si>
+    <t>Check stored procedure
+"SelectAllCustomersByCity" by passing 'cityname' as input parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHOW PROCEDURE STATUS 
+WHERE db= 'classicmodels';
+OR
+SHOW PROCEDURE STATUS 
+WHERE Name= 'SelectAllCustomers';
+</t>
+  </si>
+  <si>
+    <t>Test Query</t>
+  </si>
+  <si>
+    <t>call SelectAllCustomers();</t>
+  </si>
+  <si>
+    <t>call SelectAllCustomersByCity('Singapore');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) CALL GetCustomerShipping(112, @shipping);
+SELECT @shipping AS ShippingTime;
+2) CALL GetCustomerShipping(260, @shipping);
+SELECT @shipping AS ShippingTime;
+3) CALL GetCustomerShipping(353, @shipping);
+SELECT @shipping AS ShippingTime;
+</t>
+  </si>
+  <si>
+    <t>SELECT * FROM customers;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM customers
+WHERE city = 'Singapore';</t>
+  </si>
+  <si>
+    <t>SELECT * FROM customers</t>
+  </si>
+  <si>
+    <t>SELECT country, 
+  CASE 
+   WHEN country='USA' THEN 
+                  '2-day Shipping'
+   WHEN country='Canada' THEN
+                  '3-day Shipping'
+   ELSE      '5-day Shipping'
+  END AS ShippingTime
+  FROM customers
+  WHERE customerNumber=112;</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>SP name should be displayed in the list</t>
+  </si>
+  <si>
+    <t>City Name: Singapore</t>
+  </si>
+  <si>
+    <t>City Name: Singapore
+PinCode:079903</t>
+  </si>
+  <si>
+    <t>CustId: 141</t>
+  </si>
+  <si>
+    <t>CustId: 112
+CustId: 260
+CustId: 353</t>
+  </si>
+  <si>
+    <t>Display all records from the 'Customers' table</t>
+  </si>
+  <si>
+    <t>Display Customers from a particular City from the Customers table</t>
+  </si>
+  <si>
+    <t>Accepts customer number and returns the total number of orders
+that were shipped, canceled, resolved, disputed</t>
+  </si>
+  <si>
+    <t>Display Customers from a particular City and a particular PostalCode
+from the Customers table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ER1: 2-day Shipping
+ER2: 3-day Shipping
+ER3: 5-day Shipping
+</t>
+  </si>
+  <si>
+    <t>SELECT * FROM customers
+WHERE city = 'Singapore' AND postalCode='079903';</t>
+  </si>
+  <si>
+    <t>call SelectAllCustomersByCityAndPCode('Singapore','079903');</t>
+  </si>
+  <si>
+    <t>call get_order_by_customer(141,@shipped,@canceled,@resolved,@disputed);
+SELECT @shipped,@canceled,@resolved,@disputed;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT
+(SELECT count(*) AS 'shipped'
+FROM orders
+WHERE customerNumber=141 AND status='Shipped') as Shipped,
+(SELECT count(*) AS 'canceled'
+FROM orders
+WHERE customerNumber=141 AND status='Canceled') as Canceled,
+(SELECT count(*) AS 'resolved'
+FROM orders
+WHERE customerNumber=141 AND status='Resolved') as Resolved,
+(SELECT count(*) AS 'disputed'
+FROM orders
+WHERE customerNumber=141 AND status='Disputed') as Disputed;
+</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Check stored procedure
+"GetCustomerShipping" by passing 'custId' as input parameter</t>
+  </si>
+  <si>
+    <t>Check stored functions are existed in the DB or not</t>
+  </si>
+  <si>
+    <t>Check stored function "CustomerLevel" returns
+ customer level when it calls from SQL Statement</t>
+  </si>
+  <si>
+    <t>Check stored function "CustomerLevel" returns
+ customer level when it calls from Stored Procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHOW FUNCTION STATUS WHERE db = 'classicmodels';
+OR
+SHOW FUNCTION STATUS WHERE Name = 'CustomerLevel';
+</t>
+  </si>
+  <si>
+    <t>SELECT customerName, CustomerLevel( creditLimit)
+FROM customers;</t>
+  </si>
+  <si>
+    <t>Pre-Requiste: Create StoredProcedure "GetCustomerLevel"
+CALL GetCustomerLevel(131,@customerLevel);
+SELECT @customerLevel;</t>
+  </si>
+  <si>
+    <t>SELECT customerName, 
+CASE WHEN creditLimit &gt; 50000 THEN
+  'PLATINUM'
+ WHEN  (creditLimit &gt;= 10000 AND creditLimit &lt;= 50000) THEN
+   'GOLD'
+ WHEN  creditLimit &lt; 10000 THEN
+   'SILVER'
+ END AS customerLevel 
+FROM customers;</t>
+  </si>
+  <si>
+    <t>StoredFunction Name should be displayed in the list</t>
+  </si>
+  <si>
+    <t>Result set should contain the same data</t>
+  </si>
+  <si>
+    <t>As Per Design</t>
+  </si>
+  <si>
+    <t>SELECT customerName, 
+CASE WHEN creditLimit &gt; 50000 THEN
+  'PLATINUM'
+ WHEN  (creditLimit &gt;= 10000 AND creditLimit &lt;= 50000) THEN
+   'GOLD'
+ WHEN  creditLimit &lt; 10000 THEN
+   'SILVER'
+ END AS customerLevel 
+FROM customers
+WHERE customerNumber=131;</t>
+  </si>
+  <si>
+    <t>Check Data Intedrity on Courses Table</t>
+  </si>
+  <si>
+    <t>Validate CourseId</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>FAILURE</t>
+  </si>
+  <si>
+    <t>Duplicate Entry Error since CourseId is PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>Validate CourseName</t>
+  </si>
+  <si>
+    <t>Duplicate Entry Error since CourseName is UNIQUE</t>
+  </si>
+  <si>
+    <t>Validate Fee</t>
+  </si>
+  <si>
+    <t>Check Constraint Violation Error since Fee is less than 100</t>
+  </si>
+  <si>
+    <t>Check Constraint Violation Error since Fee is greater than 500</t>
+  </si>
+  <si>
+    <t>Check Data Integrity on Students Table</t>
+  </si>
+  <si>
+    <t>Validate SID and SName</t>
+  </si>
+  <si>
+    <t>Validate Age</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (101, "John", 20, null, 111);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (101, "X", 20, null, 111);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (102, null, 20, null, 111);</t>
+  </si>
+  <si>
+    <t>Duplicate Entry Error since SID is PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>Column cannot be NULL ERROR since Sname is NOT NULL</t>
+  </si>
+  <si>
+    <t>Validate Doj</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Validate CourseId Forgeign Key
+(References to CourseId in Courses Table)</t>
+  </si>
+  <si>
+    <t>Delete Record from parent table
+(courses) and check child table (students)
+record automatically deleted</t>
+  </si>
+  <si>
+    <t>Check Doj column values updated automatically with 
+current date and time since it is default column</t>
+  </si>
+  <si>
+    <t>SELECT * FROM students;</t>
+  </si>
+  <si>
+    <t>DELETE FROM courses
+WHERE courseId = 222;</t>
+  </si>
+  <si>
+    <t>Record should be deleted from students</t>
+  </si>
+  <si>
+    <t>Deleting record from courses successfully</t>
+  </si>
+  <si>
+    <t>Forgein Key Constraint Error since CourseId is not available 
+in courses Table</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (104, "Scott", 30, NULL, 222);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (105, "David", 20, NULL, 555);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (102, "Smith", 15, NULL, 111);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (103, "Kim", 30, NULL, 111);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (104, "Mary", 10, NULL, 111);</t>
+  </si>
+  <si>
+    <t>INSERT INTO students ( sid, sName, age, doc, courseId )
+VALUES (104, "Mary", 35, NULL, 111);</t>
+  </si>
+  <si>
+    <t>Check Constraint Violation Error since Age is less than 15</t>
+  </si>
+  <si>
+    <t>Check Constraint Violation Error since Age is greater than 30</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 111, "Java", 3, 500 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 111, "Python", 2, 300 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( null, "Java", 2, 300 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 222, "Python", 2, 300 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 333, "Python", 2, 300 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 333, "Javascript", 1, 100 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 444, "Typescript", 1, 500 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES ( 555, "vbscript", 1, 50 );</t>
+  </si>
+  <si>
+    <t>INSERT INTO courses 
+VALUES (  555, "vbscript", 1, 600 );</t>
+  </si>
+  <si>
+    <t>SELECT doj FROM students;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,8 +601,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +640,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,17 +712,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +1091,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,24 +1362,24 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1153,29 +1596,694 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15EBC3-20DA-4AB0-933A-2F69770B93B3}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B8" sqref="A4:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="15" customFormat="1" ht="393.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="187.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B019252D-4496-4556-9804-744947BB333D}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B041DE-A901-479C-9317-30BBDA0D8101}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18A5CF9-9062-4F06-B53B-499607BA9309}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="3"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1188,17 +2296,17 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>6</v>
@@ -1209,101 +2317,568 @@
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="B16" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="D18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="C20" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="C25" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="C30" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>